<commit_message>
Se creo la clase main,en la cual se va a procesar la interaccion con el usuario final.
</commit_message>
<xml_diff>
--- a/excel/plantilla.xlsx
+++ b/excel/plantilla.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oderb\Documents\NetBeansProjects\ReconocedorRelaciones\excel\"/>
     </mc:Choice>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="5">
   <si>
     <t>PDF</t>
   </si>
@@ -55,6 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -35693,13 +35694,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35716,89 +35717,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>483133</v>
+      <c r="B2" t="n">
+        <v>483133.0</v>
       </c>
-      <c r="C2">
-        <v>5109</v>
+      <c r="C2" t="n">
+        <v>5109.0</v>
       </c>
-      <c r="D2">
-        <v>21276</v>
+      <c r="D2" t="n">
+        <v>21276.0</v>
       </c>
-      <c r="E2">
-        <v>204</v>
+      <c r="E2" t="n">
+        <v>204.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>489680</v>
+      <c r="B3" t="n">
+        <v>489680.0</v>
       </c>
-      <c r="C3">
-        <v>6547</v>
+      <c r="C3" t="n">
+        <v>6547.0</v>
       </c>
-      <c r="D3">
-        <v>21501</v>
+      <c r="D3" t="n">
+        <v>21501.0</v>
       </c>
-      <c r="E3">
-        <v>225</v>
+      <c r="E3" t="n">
+        <v>225.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>498555</v>
+      <c r="B4" t="n">
+        <v>498555.0</v>
       </c>
-      <c r="C4">
-        <v>8875</v>
+      <c r="C4" t="n">
+        <v>8875.0</v>
       </c>
-      <c r="D4">
-        <v>21713</v>
+      <c r="D4" t="n">
+        <v>21713.0</v>
       </c>
-      <c r="E4">
-        <v>212</v>
+      <c r="E4" t="n">
+        <v>212.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>507996</v>
+      <c r="B5" t="n">
+        <v>507996.0</v>
       </c>
-      <c r="C5">
-        <v>9441</v>
+      <c r="C5" t="n">
+        <v>9441.0</v>
       </c>
-      <c r="D5">
-        <v>25648</v>
+      <c r="D5" t="n">
+        <v>25648.0</v>
       </c>
-      <c r="E5">
-        <v>3935</v>
+      <c r="E5" t="n">
+        <v>3935.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>516296</v>
+      <c r="B6" t="n">
+        <v>516296.0</v>
       </c>
-      <c r="C6">
-        <v>8300</v>
+      <c r="C6" t="n">
+        <v>8300.0</v>
       </c>
-      <c r="D6">
-        <v>25856</v>
+      <c r="D6" t="n">
+        <v>25856.0</v>
       </c>
-      <c r="E6">
-        <v>208</v>
+      <c r="E6" t="n">
+        <v>208.0</v>
       </c>
     </row>
   </sheetData>
@@ -35818,14 +35819,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35842,89 +35843,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>57966</v>
+      <c r="B2" t="n">
+        <v>57966.0</v>
       </c>
-      <c r="C2">
-        <v>979</v>
+      <c r="C2" t="n">
+        <v>979.0</v>
       </c>
-      <c r="D2">
-        <v>2233</v>
+      <c r="D2" t="n">
+        <v>2233.0</v>
       </c>
-      <c r="E2">
-        <v>11</v>
+      <c r="E2" t="n">
+        <v>11.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>59089</v>
+      <c r="B3" t="n">
+        <v>59089.0</v>
       </c>
-      <c r="C3">
-        <v>1123</v>
+      <c r="C3" t="n">
+        <v>1123.0</v>
       </c>
-      <c r="D3">
-        <v>2267</v>
+      <c r="D3" t="n">
+        <v>2267.0</v>
       </c>
-      <c r="E3">
-        <v>34</v>
+      <c r="E3" t="n">
+        <v>34.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>60284</v>
+      <c r="B4" t="n">
+        <v>60284.0</v>
       </c>
-      <c r="C4">
-        <v>1195</v>
+      <c r="C4" t="n">
+        <v>1195.0</v>
       </c>
-      <c r="D4">
-        <v>2296</v>
+      <c r="D4" t="n">
+        <v>2296.0</v>
       </c>
-      <c r="E4">
-        <v>29</v>
+      <c r="E4" t="n">
+        <v>29.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>61428</v>
+      <c r="B5" t="n">
+        <v>61428.0</v>
       </c>
-      <c r="C5">
-        <v>1144</v>
+      <c r="C5" t="n">
+        <v>1144.0</v>
       </c>
-      <c r="D5">
-        <v>2341</v>
+      <c r="D5" t="n">
+        <v>2341.0</v>
       </c>
-      <c r="E5">
-        <v>45</v>
+      <c r="E5" t="n">
+        <v>45.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>62313</v>
+      <c r="B6" t="n">
+        <v>62313.0</v>
       </c>
-      <c r="C6">
-        <v>885</v>
+      <c r="C6" t="n">
+        <v>885.0</v>
       </c>
-      <c r="D6">
-        <v>2355</v>
+      <c r="D6" t="n">
+        <v>2355.0</v>
       </c>
-      <c r="E6">
-        <v>14</v>
+      <c r="E6" t="n">
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>
@@ -35943,13 +35944,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35966,89 +35967,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>397623</v>
+      <c r="B2" t="n">
+        <v>397623.0</v>
       </c>
-      <c r="C2">
-        <v>10142</v>
+      <c r="C2" t="n">
+        <v>10142.0</v>
       </c>
-      <c r="D2">
-        <v>13154</v>
+      <c r="D2" t="n">
+        <v>13154.0</v>
       </c>
-      <c r="E2">
-        <v>312</v>
+      <c r="E2" t="n">
+        <v>312.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>410453</v>
+      <c r="B3" t="n">
+        <v>410453.0</v>
       </c>
-      <c r="C3">
-        <v>12830</v>
+      <c r="C3" t="n">
+        <v>12830.0</v>
       </c>
-      <c r="D3">
-        <v>13475</v>
+      <c r="D3" t="n">
+        <v>13475.0</v>
       </c>
-      <c r="E3">
-        <v>321</v>
+      <c r="E3" t="n">
+        <v>321.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>422519</v>
+      <c r="B4" t="n">
+        <v>422519.0</v>
       </c>
-      <c r="C4">
-        <v>12066</v>
+      <c r="C4" t="n">
+        <v>12066.0</v>
       </c>
-      <c r="D4">
-        <v>13837</v>
+      <c r="D4" t="n">
+        <v>13837.0</v>
       </c>
-      <c r="E4">
-        <v>362</v>
+      <c r="E4" t="n">
+        <v>362.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>433805</v>
+      <c r="B5" t="n">
+        <v>433805.0</v>
       </c>
-      <c r="C5">
-        <v>11286</v>
+      <c r="C5" t="n">
+        <v>11286.0</v>
       </c>
-      <c r="D5">
-        <v>14145</v>
+      <c r="D5" t="n">
+        <v>14145.0</v>
       </c>
-      <c r="E5">
-        <v>308</v>
+      <c r="E5" t="n">
+        <v>308.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>445111</v>
+      <c r="B6" t="n">
+        <v>445111.0</v>
       </c>
-      <c r="C6">
-        <v>11306</v>
+      <c r="C6" t="n">
+        <v>11306.0</v>
       </c>
-      <c r="D6">
-        <v>14492</v>
+      <c r="D6" t="n">
+        <v>14492.0</v>
       </c>
-      <c r="E6">
-        <v>347</v>
+      <c r="E6" t="n">
+        <v>347.0</v>
       </c>
     </row>
   </sheetData>
@@ -36059,7 +36060,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB13" sqref="AB13"/>
@@ -36067,18 +36068,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.85546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="2.5703125" collapsed="false"/>
+    <col min="7" max="8" customWidth="true" hidden="true" width="9.140625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="8.42578125" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" hidden="true" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36095,89 +36096,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>376616</v>
+      <c r="B2" t="n">
+        <v>376616.0</v>
       </c>
-      <c r="C2">
-        <v>1572</v>
+      <c r="C2" t="n">
+        <v>1572.0</v>
       </c>
-      <c r="D2">
-        <v>10178</v>
+      <c r="D2" t="n">
+        <v>10178.0</v>
       </c>
-      <c r="E2">
-        <v>39</v>
+      <c r="E2" t="n">
+        <v>39.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>378168</v>
+      <c r="B3" t="n">
+        <v>378168.0</v>
       </c>
-      <c r="C3">
-        <v>1552</v>
+      <c r="C3" t="n">
+        <v>1552.0</v>
       </c>
-      <c r="D3">
-        <v>10205</v>
+      <c r="D3" t="n">
+        <v>10205.0</v>
       </c>
-      <c r="E3">
-        <v>27</v>
+      <c r="E3" t="n">
+        <v>27.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>380034</v>
+      <c r="B4" t="n">
+        <v>380034.0</v>
       </c>
-      <c r="C4">
-        <v>1866</v>
+      <c r="C4" t="n">
+        <v>1866.0</v>
       </c>
-      <c r="D4">
-        <v>10299</v>
+      <c r="D4" t="n">
+        <v>10299.0</v>
       </c>
-      <c r="E4">
-        <v>94</v>
+      <c r="E4" t="n">
+        <v>94.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>382111</v>
+      <c r="B5" t="n">
+        <v>382111.0</v>
       </c>
-      <c r="C5">
-        <v>2077</v>
+      <c r="C5" t="n">
+        <v>2077.0</v>
       </c>
-      <c r="D5">
-        <v>10340</v>
+      <c r="D5" t="n">
+        <v>10340.0</v>
       </c>
-      <c r="E5">
-        <v>41</v>
+      <c r="E5" t="n">
+        <v>41.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>383902</v>
+      <c r="B6" t="n">
+        <v>383902.0</v>
       </c>
-      <c r="C6">
-        <v>1791</v>
+      <c r="C6" t="n">
+        <v>1791.0</v>
       </c>
-      <c r="D6">
-        <v>10395</v>
+      <c r="D6" t="n">
+        <v>10395.0</v>
       </c>
-      <c r="E6">
-        <v>55</v>
+      <c r="E6" t="n">
+        <v>55.0</v>
       </c>
     </row>
   </sheetData>
@@ -36196,7 +36197,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36213,89 +36214,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>253868</v>
+      <c r="B2" t="n">
+        <v>253868.0</v>
       </c>
-      <c r="C2">
-        <v>7369</v>
+      <c r="C2" t="n">
+        <v>7369.0</v>
       </c>
-      <c r="D2">
-        <v>4785</v>
+      <c r="D2" t="n">
+        <v>4785.0</v>
       </c>
-      <c r="E2">
-        <v>151</v>
+      <c r="E2" t="n">
+        <v>151.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>260911</v>
+      <c r="B3" t="n">
+        <v>260911.0</v>
       </c>
-      <c r="C3">
-        <v>7043</v>
+      <c r="C3" t="n">
+        <v>7043.0</v>
       </c>
-      <c r="D3">
-        <v>5088</v>
+      <c r="D3" t="n">
+        <v>5088.0</v>
       </c>
-      <c r="E3">
-        <v>303</v>
+      <c r="E3" t="n">
+        <v>303.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>268574</v>
+      <c r="B4" t="n">
+        <v>268574.0</v>
       </c>
-      <c r="C4">
-        <v>7663</v>
+      <c r="C4" t="n">
+        <v>7663.0</v>
       </c>
-      <c r="D4">
-        <v>5246</v>
+      <c r="D4" t="n">
+        <v>5246.0</v>
       </c>
-      <c r="E4">
-        <v>158</v>
+      <c r="E4" t="n">
+        <v>158.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>276072</v>
+      <c r="B5" t="n">
+        <v>276072.0</v>
       </c>
-      <c r="C5">
-        <v>7498</v>
+      <c r="C5" t="n">
+        <v>7498.0</v>
       </c>
-      <c r="D5">
-        <v>5428</v>
+      <c r="D5" t="n">
+        <v>5428.0</v>
       </c>
-      <c r="E5">
-        <v>182</v>
+      <c r="E5" t="n">
+        <v>182.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>282437</v>
+      <c r="B6" t="n">
+        <v>282437.0</v>
       </c>
-      <c r="C6">
-        <v>6365</v>
+      <c r="C6" t="n">
+        <v>6365.0</v>
       </c>
-      <c r="D6">
-        <v>5565</v>
+      <c r="D6" t="n">
+        <v>5565.0</v>
       </c>
-      <c r="E6">
-        <v>137</v>
+      <c r="E6" t="n">
+        <v>137.0</v>
       </c>
     </row>
   </sheetData>
@@ -36314,7 +36315,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36331,89 +36332,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>120132</v>
+      <c r="B2" t="n">
+        <v>120132.0</v>
       </c>
-      <c r="C2">
-        <v>681</v>
+      <c r="C2" t="n">
+        <v>681.0</v>
       </c>
-      <c r="D2">
-        <v>8987</v>
+      <c r="D2" t="n">
+        <v>8987.0</v>
       </c>
-      <c r="E2">
-        <v>6</v>
+      <c r="E2" t="n">
+        <v>6.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>120421</v>
+      <c r="B3" t="n">
+        <v>120421.0</v>
       </c>
-      <c r="C3">
-        <v>289</v>
+      <c r="C3" t="n">
+        <v>289.0</v>
       </c>
-      <c r="D3">
-        <v>8991</v>
+      <c r="D3" t="n">
+        <v>8991.0</v>
       </c>
-      <c r="E3">
-        <v>4</v>
+      <c r="E3" t="n">
+        <v>4.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>120844</v>
+      <c r="B4" t="n">
+        <v>120844.0</v>
       </c>
-      <c r="C4">
-        <v>423</v>
+      <c r="C4" t="n">
+        <v>423.0</v>
       </c>
-      <c r="D4">
-        <v>9006</v>
+      <c r="D4" t="n">
+        <v>9006.0</v>
       </c>
-      <c r="E4">
-        <v>15</v>
+      <c r="E4" t="n">
+        <v>15.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>121234</v>
+      <c r="B5" t="n">
+        <v>121234.0</v>
       </c>
-      <c r="C5">
-        <v>390</v>
+      <c r="C5" t="n">
+        <v>390.0</v>
       </c>
-      <c r="D5">
-        <v>9015</v>
+      <c r="D5" t="n">
+        <v>9015.0</v>
       </c>
-      <c r="E5">
-        <v>9</v>
+      <c r="E5" t="n">
+        <v>9.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>121652</v>
+      <c r="B6" t="n">
+        <v>121652.0</v>
       </c>
-      <c r="C6">
-        <v>418</v>
+      <c r="C6" t="n">
+        <v>418.0</v>
       </c>
-      <c r="D6">
-        <v>9020</v>
+      <c r="D6" t="n">
+        <v>9020.0</v>
       </c>
-      <c r="E6">
-        <v>5</v>
+      <c r="E6" t="n">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>
@@ -36432,7 +36433,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36449,89 +36450,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>95563</v>
+      <c r="B2" t="n">
+        <v>95563.0</v>
       </c>
-      <c r="C2">
-        <v>862</v>
+      <c r="C2" t="n">
+        <v>862.0</v>
       </c>
-      <c r="D2">
-        <v>5951</v>
+      <c r="D2" t="n">
+        <v>5951.0</v>
       </c>
-      <c r="E2">
-        <v>19</v>
+      <c r="E2" t="n">
+        <v>19.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>95563</v>
+      <c r="B3" t="n">
+        <v>95563.0</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="n">
+        <v>0.0</v>
       </c>
-      <c r="D3">
-        <v>5951</v>
+      <c r="D3" t="n">
+        <v>5951.0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="n">
+        <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>98343</v>
+      <c r="B4" t="n">
+        <v>98343.0</v>
       </c>
-      <c r="C4">
-        <v>1233</v>
+      <c r="C4" t="n">
+        <v>1233.0</v>
       </c>
-      <c r="D4">
-        <v>6010</v>
+      <c r="D4" t="n">
+        <v>6010.0</v>
       </c>
-      <c r="E4">
-        <v>26</v>
+      <c r="E4" t="n">
+        <v>26.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>99409</v>
+      <c r="B5" t="n">
+        <v>99409.0</v>
       </c>
-      <c r="C5">
-        <v>1066</v>
+      <c r="C5" t="n">
+        <v>1066.0</v>
       </c>
-      <c r="D5">
-        <v>6030</v>
+      <c r="D5" t="n">
+        <v>6030.0</v>
       </c>
-      <c r="E5">
-        <v>20</v>
+      <c r="E5" t="n">
+        <v>20.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>100688</v>
+      <c r="B6" t="n">
+        <v>100688.0</v>
       </c>
-      <c r="C6">
-        <v>1279</v>
+      <c r="C6" t="n">
+        <v>1279.0</v>
       </c>
-      <c r="D6">
-        <v>6065</v>
+      <c r="D6" t="n">
+        <v>6065.0</v>
       </c>
-      <c r="E6">
-        <v>35</v>
+      <c r="E6" t="n">
+        <v>35.0</v>
       </c>
     </row>
   </sheetData>
@@ -36550,7 +36551,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36567,89 +36568,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>91635</v>
+      <c r="B2" t="n">
+        <v>91635.0</v>
       </c>
-      <c r="C2">
-        <v>1636</v>
+      <c r="C2" t="n">
+        <v>1636.0</v>
       </c>
-      <c r="D2">
-        <v>3712</v>
+      <c r="D2" t="n">
+        <v>3712.0</v>
       </c>
-      <c r="E2">
-        <v>72</v>
+      <c r="E2" t="n">
+        <v>72.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>93328</v>
+      <c r="B3" t="n">
+        <v>93328.0</v>
       </c>
-      <c r="C3">
-        <v>1693</v>
+      <c r="C3" t="n">
+        <v>1693.0</v>
       </c>
-      <c r="D3">
-        <v>3761</v>
+      <c r="D3" t="n">
+        <v>3761.0</v>
       </c>
-      <c r="E3">
-        <v>49</v>
+      <c r="E3" t="n">
+        <v>49.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>95071</v>
+      <c r="B4" t="n">
+        <v>95071.0</v>
       </c>
-      <c r="C4">
-        <v>1743</v>
+      <c r="C4" t="n">
+        <v>1743.0</v>
       </c>
-      <c r="D4">
-        <v>3827</v>
+      <c r="D4" t="n">
+        <v>3827.0</v>
       </c>
-      <c r="E4">
-        <v>66</v>
+      <c r="E4" t="n">
+        <v>66.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>96459</v>
+      <c r="B5" t="n">
+        <v>96459.0</v>
       </c>
-      <c r="C5">
-        <v>1388</v>
+      <c r="C5" t="n">
+        <v>1388.0</v>
       </c>
-      <c r="D5">
-        <v>3884</v>
+      <c r="D5" t="n">
+        <v>3884.0</v>
       </c>
-      <c r="E5">
-        <v>57</v>
+      <c r="E5" t="n">
+        <v>57.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>97950</v>
+      <c r="B6" t="n">
+        <v>97950.0</v>
       </c>
-      <c r="C6">
-        <v>1491</v>
+      <c r="C6" t="n">
+        <v>1491.0</v>
       </c>
-      <c r="D6">
-        <v>3939</v>
+      <c r="D6" t="n">
+        <v>3939.0</v>
       </c>
-      <c r="E6">
-        <v>55</v>
+      <c r="E6" t="n">
+        <v>55.0</v>
       </c>
     </row>
   </sheetData>
@@ -36668,7 +36669,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36685,89 +36686,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>81094</v>
+      <c r="B2" t="n">
+        <v>81094.0</v>
       </c>
-      <c r="C2">
-        <v>595</v>
+      <c r="C2" t="n">
+        <v>595.0</v>
       </c>
-      <c r="D2">
-        <v>1346</v>
+      <c r="D2" t="n">
+        <v>1346.0</v>
       </c>
-      <c r="E2">
-        <v>18</v>
+      <c r="E2" t="n">
+        <v>18.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>82224</v>
+      <c r="B3" t="n">
+        <v>82224.0</v>
       </c>
-      <c r="C3">
-        <v>1130</v>
+      <c r="C3" t="n">
+        <v>1130.0</v>
       </c>
-      <c r="D3">
-        <v>1371</v>
+      <c r="D3" t="n">
+        <v>1371.0</v>
       </c>
-      <c r="E3">
-        <v>25</v>
+      <c r="E3" t="n">
+        <v>25.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>83134</v>
+      <c r="B4" t="n">
+        <v>83134.0</v>
       </c>
-      <c r="C4">
-        <v>910</v>
+      <c r="C4" t="n">
+        <v>910.0</v>
       </c>
-      <c r="D4">
-        <v>1393</v>
+      <c r="D4" t="n">
+        <v>1393.0</v>
       </c>
-      <c r="E4">
-        <v>22</v>
+      <c r="E4" t="n">
+        <v>22.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>84488</v>
+      <c r="B5" t="n">
+        <v>84488.0</v>
       </c>
-      <c r="C5">
-        <v>1354</v>
+      <c r="C5" t="n">
+        <v>1354.0</v>
       </c>
-      <c r="D5">
-        <v>1409</v>
+      <c r="D5" t="n">
+        <v>1409.0</v>
       </c>
-      <c r="E5">
-        <v>16</v>
+      <c r="E5" t="n">
+        <v>16.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>85545</v>
+      <c r="B6" t="n">
+        <v>85545.0</v>
       </c>
-      <c r="C6">
-        <v>1057</v>
+      <c r="C6" t="n">
+        <v>1057.0</v>
       </c>
-      <c r="D6">
-        <v>1438</v>
+      <c r="D6" t="n">
+        <v>1438.0</v>
       </c>
-      <c r="E6">
-        <v>29</v>
+      <c r="E6" t="n">
+        <v>29.0</v>
       </c>
     </row>
   </sheetData>
@@ -36786,7 +36787,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36803,89 +36804,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12.0</v>
       </c>
-      <c r="B2">
-        <v>75394</v>
+      <c r="B2" t="n">
+        <v>75394.0</v>
       </c>
-      <c r="C2">
-        <v>902</v>
+      <c r="C2" t="n">
+        <v>902.0</v>
       </c>
-      <c r="D2">
-        <v>1664</v>
+      <c r="D2" t="n">
+        <v>1664.0</v>
       </c>
-      <c r="E2">
-        <v>25</v>
+      <c r="E2" t="n">
+        <v>25.0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>13.0</v>
       </c>
-      <c r="B3">
-        <v>76464</v>
+      <c r="B3" t="n">
+        <v>76464.0</v>
       </c>
-      <c r="C3">
-        <v>1070</v>
+      <c r="C3" t="n">
+        <v>1070.0</v>
       </c>
-      <c r="D3">
-        <v>1680</v>
+      <c r="D3" t="n">
+        <v>1680.0</v>
       </c>
-      <c r="E3">
-        <v>16</v>
+      <c r="E3" t="n">
+        <v>16.0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>14</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14.0</v>
       </c>
-      <c r="B4">
-        <v>77377</v>
+      <c r="B4" t="n">
+        <v>77377.0</v>
       </c>
-      <c r="C4">
-        <v>913</v>
+      <c r="C4" t="n">
+        <v>913.0</v>
       </c>
-      <c r="D4">
-        <v>1703</v>
+      <c r="D4" t="n">
+        <v>1703.0</v>
       </c>
-      <c r="E4">
-        <v>23</v>
+      <c r="E4" t="n">
+        <v>23.0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15.0</v>
       </c>
-      <c r="B5">
-        <v>78446</v>
+      <c r="B5" t="n">
+        <v>78446.0</v>
       </c>
-      <c r="C5">
-        <v>1069</v>
+      <c r="C5" t="n">
+        <v>1069.0</v>
       </c>
-      <c r="D5">
-        <v>1722</v>
+      <c r="D5" t="n">
+        <v>1722.0</v>
       </c>
-      <c r="E5">
-        <v>19</v>
+      <c r="E5" t="n">
+        <v>19.0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>16</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16.0</v>
       </c>
-      <c r="B6">
-        <v>79402</v>
+      <c r="B6" t="n">
+        <v>79402.0</v>
       </c>
-      <c r="C6">
-        <v>956</v>
+      <c r="C6" t="n">
+        <v>956.0</v>
       </c>
-      <c r="D6">
-        <v>1734</v>
+      <c r="D6" t="n">
+        <v>1734.0</v>
       </c>
-      <c r="E6">
-        <v>12</v>
+      <c r="E6" t="n">
+        <v>12.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>